<commit_message>
Look at both worksheet autofilter as well as table autofilters to determine to leave space for arrow
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -460,9 +460,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="8.090625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="10.805425" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.860625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.170625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.665425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="9.830625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -572,9 +572,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="8.090625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="10.805425" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.860625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.170625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.665425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="9.830625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -684,9 +684,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="8.090625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="10.805425" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.860625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.170625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="10.665425" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="9.830625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>

<commit_message>
Reference files updated (minor changes in XML: items reordered, default style elements skipped)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -126,34 +126,12 @@
   </x:cellStyles>
   <x:dxfs count="1">
     <x:dxf>
-      <x:font>
-        <x:vertAlign val="baseline"/>
-        <x:sz val="11"/>
-        <x:color rgb="FF000000"/>
-        <x:name val="Calibri"/>
-        <x:family val="2"/>
-      </x:font>
+      <x:font/>
       <x:numFmt numFmtId="14" formatCode="M/d/yyyy"/>
       <x:fill>
         <x:patternFill patternType="none"/>
       </x:fill>
-      <x:border diagonalUp="0" diagonalDown="0">
-        <x:left style="none">
-          <x:color rgb="FF000000"/>
-        </x:left>
-        <x:right style="none">
-          <x:color rgb="FF000000"/>
-        </x:right>
-        <x:top style="none">
-          <x:color rgb="FF000000"/>
-        </x:top>
-        <x:bottom style="none">
-          <x:color rgb="FF000000"/>
-        </x:bottom>
-        <x:diagonal style="none">
-          <x:color rgb="FF000000"/>
-        </x:diagonal>
-      </x:border>
+      <x:border/>
     </x:dxf>
   </x:dxfs>
 </x:styleSheet>

</xml_diff>

<commit_message>
Change XLTable.Theme default value to TableStyleMedium2 to align with Excel
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -144,7 +144,7 @@
     <x:tableColumn id="3" name="Patient"/>
     <x:tableColumn id="4" name="Date" dataDxfId="0"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -157,7 +157,7 @@
     <x:tableColumn id="3" name="Patient"/>
     <x:tableColumn id="4" name="Date" dataDxfId="0"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -170,7 +170,7 @@
     <x:tableColumn id="3" name="Patient"/>
     <x:tableColumn id="4" name="Date" dataDxfId="0"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 

</xml_diff>

<commit_message>
Make default table name equal to sheet name
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/AddingDataSet.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Patients" displayName="Patients" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Employees" displayName="Employees" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D6" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Information" displayName="Information" ref="A1:D6" totalsRowShown="0">
   <x:autoFilter ref="A1:D6"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Dosage"/>

</xml_diff>